<commit_message>
Add functions to get file suffix and file name.
</commit_message>
<xml_diff>
--- a/afm_communites_with_nova/data/test.xlsx
+++ b/afm_communites_with_nova/data/test.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="2715" windowWidth="15705" windowHeight="1950"/>
   </bookViews>
   <sheets>
     <sheet name="setpoints" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -356,10 +357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -378,6 +379,14 @@
       </c>
       <c r="B2">
         <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>